<commit_message>
Se agrego nuevo contenido
</commit_message>
<xml_diff>
--- a/5 - Diagrama de Gantt - Tareas x Tiempo/5 - Diagrama de Gantt.xlsx
+++ b/5 - Diagrama de Gantt - Tareas x Tiempo/5 - Diagrama de Gantt.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Grafico de Gantt  - Diseño de tareas - Tiempo: 3° Año 2024</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Diagrama de flujo</t>
+  </si>
+  <si>
+    <t>Correcciones y cambios</t>
   </si>
   <si>
     <t>Prototipo</t>
@@ -1551,7 +1554,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="8">
-        <v>45470.0</v>
+        <v>45474.0</v>
       </c>
       <c r="D12" s="8">
         <v>45477.0</v>
@@ -1559,7 +1562,7 @@
       <c r="E12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="11"/>
@@ -1631,14 +1634,14 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="8">
-        <v>45477.0</v>
+        <v>45470.0</v>
       </c>
       <c r="D13" s="8">
-        <v>45516.0</v>
+        <v>45477.0</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>7</v>
@@ -1722,7 +1725,7 @@
         <v>45477.0</v>
       </c>
       <c r="D14" s="8">
-        <v>45524.0</v>
+        <v>45516.0</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>7</v>
@@ -1803,10 +1806,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="8">
-        <v>45524.0</v>
+        <v>45477.0</v>
       </c>
       <c r="D15" s="8">
-        <v>45531.0</v>
+        <v>45524.0</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>7</v>
@@ -1883,14 +1886,14 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="8">
-        <v>45531.0</v>
+        <v>45524.0</v>
       </c>
       <c r="D16" s="8">
-        <v>45550.0</v>
+        <v>45531.0</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>7</v>
@@ -1971,10 +1974,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="8">
-        <v>45550.0</v>
+        <v>45531.0</v>
       </c>
       <c r="D17" s="8">
-        <v>45580.0</v>
+        <v>45550.0</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>7</v>
@@ -2055,10 +2058,10 @@
         <v>23</v>
       </c>
       <c r="C18" s="8">
-        <v>45580.0</v>
+        <v>45550.0</v>
       </c>
       <c r="D18" s="8">
-        <v>45590.0</v>
+        <v>45580.0</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>7</v>
@@ -2139,10 +2142,10 @@
         <v>24</v>
       </c>
       <c r="C19" s="8">
-        <v>45590.0</v>
+        <v>45580.0</v>
       </c>
       <c r="D19" s="8">
-        <v>45611.0</v>
+        <v>45590.0</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>7</v>
@@ -2223,10 +2226,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="8">
-        <v>45611.0</v>
+        <v>45590.0</v>
       </c>
       <c r="D20" s="8">
-        <v>45621.0</v>
+        <v>45611.0</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>7</v>
@@ -2307,10 +2310,10 @@
         <v>26</v>
       </c>
       <c r="C21" s="8">
-        <v>45621.0</v>
+        <v>45611.0</v>
       </c>
       <c r="D21" s="8">
-        <v>45631.0</v>
+        <v>45621.0</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>7</v>
@@ -2387,11 +2390,21 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="B22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="8">
+        <v>45621.0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>45631.0</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -2609,7 +2622,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="17"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
@@ -2831,7 +2844,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="14"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
@@ -3053,7 +3066,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="17"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="16"/>
@@ -3204,8 +3217,8 @@
       <c r="B33" s="17"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -3275,9 +3288,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="18" t="s">
-        <v>27</v>
-      </c>
+      <c r="B34" s="17"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -3351,7 +3362,9 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="17"/>
+      <c r="B35" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
@@ -18150,10 +18163,78 @@
       <c r="BT234" s="11"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="C235" s="19"/>
-      <c r="D235" s="19"/>
-      <c r="E235" s="19"/>
-      <c r="F235" s="19"/>
+      <c r="A235" s="1"/>
+      <c r="B235" s="17"/>
+      <c r="C235" s="15"/>
+      <c r="D235" s="15"/>
+      <c r="E235" s="15"/>
+      <c r="F235" s="15"/>
+      <c r="G235" s="11"/>
+      <c r="H235" s="11"/>
+      <c r="I235" s="11"/>
+      <c r="J235" s="11"/>
+      <c r="K235" s="11"/>
+      <c r="L235" s="11"/>
+      <c r="M235" s="11"/>
+      <c r="N235" s="11"/>
+      <c r="O235" s="11"/>
+      <c r="P235" s="11"/>
+      <c r="Q235" s="11"/>
+      <c r="R235" s="11"/>
+      <c r="S235" s="11"/>
+      <c r="T235" s="11"/>
+      <c r="U235" s="11"/>
+      <c r="V235" s="11"/>
+      <c r="W235" s="11"/>
+      <c r="X235" s="11"/>
+      <c r="Y235" s="11"/>
+      <c r="Z235" s="11"/>
+      <c r="AA235" s="11"/>
+      <c r="AB235" s="11"/>
+      <c r="AC235" s="11"/>
+      <c r="AD235" s="11"/>
+      <c r="AE235" s="11"/>
+      <c r="AF235" s="11"/>
+      <c r="AG235" s="11"/>
+      <c r="AH235" s="11"/>
+      <c r="AI235" s="11"/>
+      <c r="AJ235" s="11"/>
+      <c r="AK235" s="11"/>
+      <c r="AL235" s="11"/>
+      <c r="AM235" s="11"/>
+      <c r="AN235" s="11"/>
+      <c r="AO235" s="11"/>
+      <c r="AP235" s="11"/>
+      <c r="AQ235" s="11"/>
+      <c r="AR235" s="11"/>
+      <c r="AS235" s="11"/>
+      <c r="AT235" s="11"/>
+      <c r="AU235" s="11"/>
+      <c r="AV235" s="11"/>
+      <c r="AW235" s="11"/>
+      <c r="AX235" s="11"/>
+      <c r="AY235" s="11"/>
+      <c r="AZ235" s="11"/>
+      <c r="BA235" s="11"/>
+      <c r="BB235" s="11"/>
+      <c r="BC235" s="11"/>
+      <c r="BD235" s="11"/>
+      <c r="BE235" s="11"/>
+      <c r="BF235" s="11"/>
+      <c r="BG235" s="11"/>
+      <c r="BH235" s="11"/>
+      <c r="BI235" s="11"/>
+      <c r="BJ235" s="11"/>
+      <c r="BK235" s="11"/>
+      <c r="BL235" s="11"/>
+      <c r="BM235" s="11"/>
+      <c r="BN235" s="11"/>
+      <c r="BO235" s="11"/>
+      <c r="BP235" s="11"/>
+      <c r="BQ235" s="11"/>
+      <c r="BR235" s="11"/>
+      <c r="BS235" s="11"/>
+      <c r="BT235" s="11"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
       <c r="C236" s="19"/>
@@ -22745,32 +22826,38 @@
       <c r="E1000" s="19"/>
       <c r="F1000" s="19"/>
     </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="C1001" s="19"/>
+      <c r="D1001" s="19"/>
+      <c r="E1001" s="19"/>
+      <c r="F1001" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="L1:AH1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G3:BT1000">
+  <conditionalFormatting sqref="G3:BT1001">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(G3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:BT1000">
+  <conditionalFormatting sqref="G3:BT1001">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($C3&lt;=G$2,$D3&gt;=G$2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F3:F32">
+    <dataValidation type="list" allowBlank="1" sqref="F3:F33">
       <formula1>'Parámetros'!$B$2:$B$5</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C3:D32 C33:F1000">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C3:D33 C34:F1001">
       <formula1>OR(NOT(ISERROR(DATEVALUE(C3))), AND(ISNUMBER(C3), LEFT(CELL("format", C3))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E22:E32">
+    <dataValidation type="list" allowBlank="1" sqref="E23:E33">
       <formula1>'Parámetros'!$A$2:$A$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E3:E21">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E22">
       <formula1>'Parámetros'!$A$2:$A$35</formula1>
     </dataValidation>
   </dataValidations>
@@ -22799,23 +22886,23 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>8</v>
@@ -22823,18 +22910,18 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">

</xml_diff>